<commit_message>
11.01.2020 Mugadho Corporation Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Allocation Sheet.xlsx
+++ b/2020/Others/Allocation Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D4E6A1-6B62-4C44-BE4F-B7A46FFD6E95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCEEE4D-0FC9-4680-99C3-9E60329E3431}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>BL60</t>
   </si>
@@ -258,7 +258,16 @@
     <t xml:space="preserve">                      Address: Rozy Market, Station Bazar, Natore</t>
   </si>
   <si>
-    <t>Md Haider Khan</t>
+    <t>B24</t>
+  </si>
+  <si>
+    <t>BL98</t>
+  </si>
+  <si>
+    <t>D72</t>
+  </si>
+  <si>
+    <t>Md Kamrul Islam</t>
   </si>
 </sst>
 </file>
@@ -636,8 +645,8 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2936,13 +2945,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -2959,7 +2968,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1228725" y="809625"/>
+          <a:off x="1276350" y="809625"/>
           <a:ext cx="0" cy="342900"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3327,8 +3336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3417,7 +3426,7 @@
         <v>50</v>
       </c>
       <c r="L4" s="42" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M4" s="43"/>
     </row>
@@ -3508,11 +3517,9 @@
     </row>
     <row r="8" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="26">
-        <v>790</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B8" s="26"/>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
@@ -3531,10 +3538,10 @@
     </row>
     <row r="9" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B9" s="26">
-        <v>800</v>
+        <v>790</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="27"/>
@@ -3554,10 +3561,10 @@
     </row>
     <row r="10" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B10" s="26">
-        <v>915</v>
+        <v>800</v>
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="27"/>
@@ -3577,10 +3584,10 @@
     </row>
     <row r="11" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B11" s="26">
-        <v>845</v>
+        <v>915</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
@@ -3600,10 +3607,10 @@
     </row>
     <row r="12" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="26">
-        <v>880</v>
+        <v>845</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -3622,12 +3629,10 @@
       <c r="M12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="26">
-        <v>900</v>
-      </c>
+      <c r="A13" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="28"/>
       <c r="C13" s="27"/>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -3648,10 +3653,10 @@
     </row>
     <row r="14" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B14" s="26">
-        <v>1040</v>
+        <v>880</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -3671,10 +3676,10 @@
     </row>
     <row r="15" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B15" s="26">
-        <v>930</v>
+        <v>900</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
@@ -3694,10 +3699,10 @@
     </row>
     <row r="16" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B16" s="26">
-        <v>1190</v>
+        <v>1040</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
@@ -3717,10 +3722,10 @@
     </row>
     <row r="17" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B17" s="26">
-        <v>1170</v>
+        <v>930</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
@@ -3739,11 +3744,11 @@
       <c r="M17" s="11"/>
     </row>
     <row r="18" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="27">
-        <v>1070</v>
+      <c r="A18" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="26">
+        <v>1190</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
@@ -3763,10 +3768,10 @@
     </row>
     <row r="19" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B19" s="26">
-        <v>1100</v>
+        <v>1170</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
@@ -3785,12 +3790,10 @@
       <c r="M19" s="11"/>
     </row>
     <row r="20" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="27">
-        <v>1160</v>
-      </c>
+      <c r="A20" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="28"/>
       <c r="C20" s="27"/>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
@@ -3808,11 +3811,11 @@
       <c r="M20" s="11"/>
     </row>
     <row r="21" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="26">
-        <v>1010</v>
+      <c r="A21" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="27">
+        <v>1070</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="27"/>
@@ -3832,10 +3835,10 @@
     </row>
     <row r="22" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B22" s="26">
-        <v>970</v>
+        <v>1100</v>
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
@@ -3854,11 +3857,11 @@
       <c r="M22" s="11"/>
     </row>
     <row r="23" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="26">
-        <v>1050</v>
+      <c r="A23" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="27">
+        <v>1160</v>
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
@@ -3878,10 +3881,10 @@
     </row>
     <row r="24" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="25">
-        <v>1190</v>
+        <v>8</v>
+      </c>
+      <c r="B24" s="26">
+        <v>1010</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
@@ -3900,11 +3903,11 @@
       <c r="M24" s="11"/>
     </row>
     <row r="25" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="27">
-        <v>1100</v>
+      <c r="A25" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="26">
+        <v>970</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
@@ -3923,11 +3926,11 @@
       <c r="M25" s="11"/>
     </row>
     <row r="26" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="27">
-        <v>1250</v>
+      <c r="A26" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="26">
+        <v>1050</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
@@ -3946,11 +3949,11 @@
       <c r="S26" s="2"/>
     </row>
     <row r="27" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="27">
-        <v>1370</v>
+      <c r="A27" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="25">
+        <v>1190</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
@@ -3969,8 +3972,12 @@
       <c r="S27" s="2"/>
     </row>
     <row r="28" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
+      <c r="A28" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="27">
+        <v>1100</v>
+      </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
@@ -3986,8 +3993,12 @@
       <c r="M28" s="16"/>
     </row>
     <row r="29" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="27">
+        <v>1250</v>
+      </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
@@ -4003,8 +4014,12 @@
       <c r="M29" s="36"/>
     </row>
     <row r="30" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="27">
+        <v>1370</v>
+      </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
@@ -4265,8 +4280,8 @@
       <c r="N48" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="H7:I27">
-    <sortCondition ref="H6"/>
+  <sortState ref="A6:B30">
+    <sortCondition ref="A6"/>
   </sortState>
   <mergeCells count="15">
     <mergeCell ref="D40:I41"/>

</xml_diff>

<commit_message>
29.01.2020 Mugdho corporation Details
</commit_message>
<xml_diff>
--- a/2020/Others/Allocation Sheet.xlsx
+++ b/2020/Others/Allocation Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06FB4B5-29C9-4D6A-BB52-96EF86DB600C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E1494F-EABC-4051-8DC4-5B7061037D94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Allocation Sheet" sheetId="3" r:id="rId1"/>
@@ -267,7 +267,7 @@
     <t>D72</t>
   </si>
   <si>
-    <t>Md Haider Khan</t>
+    <t>Md Atikur Rahman</t>
   </si>
 </sst>
 </file>
@@ -648,6 +648,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -688,33 +715,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3337,7 +3337,7 @@
   <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3359,38 +3359,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
@@ -3425,10 +3425,10 @@
       <c r="K4" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="M4" s="57"/>
+      <c r="M4" s="43"/>
     </row>
     <row r="5" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -3519,7 +3519,9 @@
       <c r="A8" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="26">
+        <v>740</v>
+      </c>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
@@ -3761,7 +3763,7 @@
         <v>30</v>
       </c>
       <c r="I18" s="28">
-        <v>4550</v>
+        <v>4180</v>
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
@@ -3985,13 +3987,13 @@
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
-      <c r="H28" s="53" t="s">
+      <c r="H28" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="53"/>
+      <c r="I28" s="39"/>
       <c r="J28" s="11"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
       <c r="M28" s="16"/>
     </row>
     <row r="29" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -4006,14 +4008,14 @@
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
-      <c r="H29" s="49" t="s">
+      <c r="H29" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="50"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="36"/>
     </row>
     <row r="30" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
@@ -4033,10 +4035,10 @@
       <c r="I30" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="51"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="37"/>
     </row>
     <row r="31" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
@@ -4053,7 +4055,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
-      <c r="M31" s="51"/>
+      <c r="M31" s="37"/>
     </row>
     <row r="32" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -4070,7 +4072,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
-      <c r="M32" s="51"/>
+      <c r="M32" s="37"/>
     </row>
     <row r="33" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
@@ -4087,7 +4089,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
-      <c r="M33" s="51"/>
+      <c r="M33" s="37"/>
     </row>
     <row r="34" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
@@ -4104,7 +4106,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
       <c r="L34" s="11"/>
-      <c r="M34" s="51"/>
+      <c r="M34" s="37"/>
     </row>
     <row r="35" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
@@ -4121,7 +4123,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="11"/>
       <c r="L35" s="11"/>
-      <c r="M35" s="51"/>
+      <c r="M35" s="37"/>
     </row>
     <row r="36" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
@@ -4138,7 +4140,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
-      <c r="M36" s="51"/>
+      <c r="M36" s="37"/>
     </row>
     <row r="37" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
@@ -4155,7 +4157,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
-      <c r="M37" s="51"/>
+      <c r="M37" s="37"/>
     </row>
     <row r="38" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -4172,7 +4174,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
       <c r="L38" s="11"/>
-      <c r="M38" s="51"/>
+      <c r="M38" s="37"/>
     </row>
     <row r="39" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -4189,43 +4191,43 @@
       <c r="J39" s="11"/>
       <c r="K39" s="11"/>
       <c r="L39" s="11"/>
-      <c r="M39" s="52"/>
+      <c r="M39" s="38"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="44"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="35" t="s">
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="44"/>
       <c r="J40" s="31"/>
-      <c r="K40" s="37" t="s">
+      <c r="K40" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="L40" s="37"/>
-      <c r="M40" s="38"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="47"/>
     </row>
     <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
-      <c r="B41" s="46"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
+      <c r="A41" s="54"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
       <c r="J41" s="32"/>
-      <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
-      <c r="M41" s="40"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="49"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
@@ -4243,25 +4245,25 @@
       <c r="M42" s="20"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="41"/>
+      <c r="B43" s="50"/>
       <c r="C43" s="2"/>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
-      <c r="F43" s="47" t="s">
+      <c r="F43" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
       <c r="I43" s="18"/>
       <c r="J43" s="2"/>
-      <c r="K43" s="42" t="s">
+      <c r="K43" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="L43" s="42"/>
-      <c r="M43" s="42"/>
+      <c r="L43" s="51"/>
+      <c r="M43" s="51"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
@@ -4269,9 +4271,9 @@
       <c r="C44" s="2"/>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
       <c r="I44" s="18"/>
       <c r="J44" s="2"/>
       <c r="K44" s="18"/>
@@ -4286,6 +4288,13 @@
     <sortCondition ref="A6"/>
   </sortState>
   <mergeCells count="15">
+    <mergeCell ref="D40:I41"/>
+    <mergeCell ref="K40:M41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="A40:C41"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:H44"/>
     <mergeCell ref="H29:L29"/>
     <mergeCell ref="M29:M39"/>
     <mergeCell ref="J30:L30"/>
@@ -4294,13 +4303,6 @@
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D40:I41"/>
-    <mergeCell ref="K40:M41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="A40:C41"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:H44"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>

</xml_diff>